<commit_message>
Update edited session - 2025-08-26T09:54:46.167Z - Cache Bust ID: 1756202086167m5k74571m
</commit_message>
<xml_diff>
--- a/log_history/Y5_B2425_Pediatrics_checklist1756201928427_b238c595b84321b35b8e57610c49523d4e3b9b5b5d090923e9e54f4b929bedba.xlsx
+++ b/log_history/Y5_B2425_Pediatrics_checklist1756201928427_b238c595b84321b35b8e57610c49523d4e3b9b5b5d090923e9e54f4b929bedba.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Checklist" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -456,7 +456,7 @@
         <v>12:53:42</v>
       </c>
       <c r="E3" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F3" t="str">
         <v>user@user.com</v>
@@ -464,7 +464,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>201566</v>
+        <v>201559</v>
       </c>
       <c r="B4" t="str">
         <v>Pediatrics</v>
@@ -473,10 +473,10 @@
         <v>26/08/2025</v>
       </c>
       <c r="D4" t="str">
-        <v>12:53:43</v>
+        <v>12:53:44</v>
       </c>
       <c r="E4" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F4" t="str">
         <v>user@user.com</v>
@@ -484,7 +484,7 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>201559</v>
+        <v>201579</v>
       </c>
       <c r="B5" t="str">
         <v>Pediatrics</v>
@@ -493,38 +493,18 @@
         <v>26/08/2025</v>
       </c>
       <c r="D5" t="str">
-        <v>12:53:44</v>
+        <v>12:53:46</v>
       </c>
       <c r="E5" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F5" t="str">
-        <v>user@user.com</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>201579</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Pediatrics</v>
-      </c>
-      <c r="C6" t="str">
-        <v>26/08/2025</v>
-      </c>
-      <c r="D6" t="str">
-        <v>12:53:46</v>
-      </c>
-      <c r="E6" t="str">
-        <v>Selection</v>
-      </c>
-      <c r="F6" t="str">
         <v>user@user.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>